<commit_message>
Updated changed LED pins
changed pin mappings in the set up funciton
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping-Correction.xlsx
+++ b/Docs/GPIO-Mapping-Correction.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Othniel\Google Drive\3rd year\Embedded project, 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttche\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Purpose</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>A8,A7,A10, C3-11, E0-3</t>
+  </si>
+  <si>
+    <t>A11, A12</t>
+  </si>
+  <si>
+    <t>DO NOT USE!!!</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +288,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -316,6 +334,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,20 +658,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -729,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -756,13 +778,13 @@
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="S3" s="10"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -796,7 +818,7 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -830,7 +852,7 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -864,7 +886,7 @@
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -898,7 +920,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -913,7 +935,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -928,7 +950,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -940,7 +962,7 @@
       </c>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -955,7 +977,7 @@
       </c>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -971,7 +993,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -986,7 +1008,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1023,7 @@
       </c>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1015,6 +1037,17 @@
         <v>41</v>
       </c>
       <c r="E15" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1028,7 +1061,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
many commits (take a cup of coffee and relax :) ) mode LED bug: fixed freestyle instrument LED update: fixed UIUdate structure modified: removed the busy wait while loops for modes and used switch cases Added Tempo to screen in composer mode: still need to get the correct tempo from Othniel Modified the update cases resetLEDs variables in Utils: needed when changing mode GPIOC_0 was not configured: so it was done done :)
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping-Correction.xlsx
+++ b/Docs/GPIO-Mapping-Correction.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttche\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\EEE3074W,2016\Project\ST080\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,17 +661,17 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -751,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -818,7 +818,7 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -886,7 +886,7 @@
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -935,7 +935,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -962,7 +962,7 @@
       </c>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="E15" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
@@ -1061,7 +1061,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>